<commit_message>
0.0.2: Enable nullable parameter for actions functions.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoPiniaActionsStructure.xlsx
+++ b/meta/program/BlancoPiniaActionsStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoPinia/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6966778-659A-DE4F-A763-EE72756397A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0920A3-F28A-F940-83FE-98F9CA8959F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="500" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,21 +332,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>value</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>constArg</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>変更不可変数かどうか</t>
-    <rPh sb="0" eb="4">
-      <t xml:space="preserve">ヘンコウフカ </t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t xml:space="preserve">ヘンスウ </t>
-    </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -399,6 +385,14 @@
     <rPh sb="0" eb="3">
       <t xml:space="preserve">ヒドウキ </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>nullable</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>nullableかどうか</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1355,7 +1349,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1407,7 +1401,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
@@ -1420,7 +1414,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="12"/>
@@ -1433,7 +1427,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -1750,7 +1744,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>62</v>
@@ -1759,7 +1753,7 @@
         <v>63</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F33" s="43"/>
       <c r="G33"/>
@@ -1770,7 +1764,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" s="42" t="s">
         <v>62</v>
@@ -1779,7 +1773,7 @@
         <v>63</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F34" s="43"/>
       <c r="G34"/>
@@ -1790,7 +1784,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C35" s="42" t="s">
         <v>62</v>
@@ -1799,7 +1793,7 @@
         <v>63</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F35" s="43"/>
       <c r="G35"/>
@@ -1810,7 +1804,7 @@
         <v>10</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="42" t="s">
         <v>62</v>
@@ -1819,7 +1813,7 @@
         <v>63</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F36" s="43"/>
       <c r="G36"/>
@@ -1976,7 +1970,7 @@
         <v>19</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="42" t="s">
         <v>62</v>
@@ -1985,7 +1979,7 @@
         <v>63</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F45" s="43"/>
       <c r="G45"/>

</xml_diff>